<commit_message>
Segunda version, con la cochinada de bd nueva
</commit_message>
<xml_diff>
--- a/Archivos/archivo_656a51bf3ac9f.xlsx
+++ b/Archivos/archivo_656a51bf3ac9f.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lalo_\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Proyect-CFE-2.0\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789CD670-BC67-4F84-90E3-E84664415402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4445DE9-E996-430C-9E80-13F5C73E4C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" tabRatio="513" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -940,46 +940,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -1000,11 +973,38 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1527,11 +1527,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:Q178"/>
+  <dimension ref="B2:G178"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="15.05"/>
@@ -1547,64 +1547,64 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" s="2" customFormat="1" ht="27.8" customHeight="1">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
       <c r="F2" s="17"/>
       <c r="G2" s="18"/>
     </row>
     <row r="3" spans="2:7" s="2" customFormat="1" ht="28.5" customHeight="1">
-      <c r="B3" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
+      <c r="B3" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="2:7" s="2" customFormat="1" ht="38.299999999999997" customHeight="1">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="25" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="2:7" s="2" customFormat="1" ht="21.8" customHeight="1">
       <c r="B5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="2:7" s="2" customFormat="1" ht="20.95" customHeight="1">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="17"/>
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="2:7" s="2" customFormat="1" ht="20.95" customHeight="1">
-      <c r="B7" s="20"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="2:7" s="2" customFormat="1" ht="20.95" customHeight="1">
       <c r="B8" s="9" t="s">
@@ -4668,13 +4668,13 @@
       </c>
     </row>
     <row r="172" spans="2:7" ht="42.75" customHeight="1">
-      <c r="B172" s="39" t="s">
+      <c r="B172" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C172" s="40"/>
-      <c r="D172" s="40"/>
-      <c r="E172" s="40"/>
-      <c r="F172" s="40"/>
+      <c r="C172" s="22"/>
+      <c r="D172" s="22"/>
+      <c r="E172" s="22"/>
+      <c r="F172" s="22"/>
       <c r="G172" s="13">
         <f>SUM(G9:G171)</f>
         <v>1609110.2312576526</v>

</xml_diff>